<commit_message>
Update DR# 635 AllHome Kawayan (Javelin DNA Pro with MS)_02_01_2021.xlsx
</commit_message>
<xml_diff>
--- a/DR# 635 AllHome Kawayan (Javelin DNA Pro with MS)_02_01_2021.xlsx
+++ b/DR# 635 AllHome Kawayan (Javelin DNA Pro with MS)_02_01_2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UBIVELOX\Documents\GitHub\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9AF1D5F-472B-42B4-9BAE-68D50673D162}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721E4229-F1E9-4782-AC08-B9D361E3C125}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1370,7 +1370,7 @@
   <dimension ref="A2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>